<commit_message>
refactor to address issues resulting in bloated fees
</commit_message>
<xml_diff>
--- a/backend/checkpoints/polygon-ETH-TEL-8.xlsx
+++ b/backend/checkpoints/polygon-ETH-TEL-8.xlsx
@@ -726,7 +726,7 @@
         <v>0.000626812114799885</v>
       </c>
       <c r="G10" t="str">
-        <v>659.19</v>
+        <v>596.81</v>
       </c>
     </row>
     <row r="11">
@@ -907,10 +907,10 @@
         <v>3244022279652375</v>
       </c>
       <c r="F18" t="str">
-        <v>0.003112110290341964</v>
+        <v>0.003209645145741389</v>
       </c>
       <c r="G18" t="str">
-        <v>5636.71</v>
+        <v>5681.33</v>
       </c>
     </row>
     <row r="19">
@@ -956,7 +956,7 @@
         <v>0.001147927185886458</v>
       </c>
       <c r="G20" t="str">
-        <v>497.75</v>
+        <v>1131.44</v>
       </c>
     </row>
     <row r="21">
@@ -976,10 +976,10 @@
         <v>0</v>
       </c>
       <c r="F21" t="str">
-        <v>21.369406418871072081</v>
+        <v>0.004616475810352206</v>
       </c>
       <c r="G21" t="str">
-        <v>10284601.83</v>
+        <v>461.03</v>
       </c>
     </row>
     <row r="22">
@@ -999,10 +999,10 @@
         <v>0</v>
       </c>
       <c r="F22" t="str">
-        <v>0.022550285841492871</v>
+        <v>0.018195551574008137</v>
       </c>
       <c r="G22" t="str">
-        <v>9865.22</v>
+        <v>4283.45</v>
       </c>
     </row>
     <row r="23">
@@ -1022,10 +1022,10 @@
         <v>0</v>
       </c>
       <c r="F23" t="str">
-        <v>0.681981210603713378</v>
+        <v>0.009707932720953876</v>
       </c>
       <c r="G23" t="str">
-        <v>689041.32</v>
+        <v>11869.79</v>
       </c>
     </row>
     <row r="24">
@@ -1045,10 +1045,10 @@
         <v>0</v>
       </c>
       <c r="F24" t="str">
-        <v>0</v>
+        <v>0.00287701430496335</v>
       </c>
       <c r="G24" t="str">
-        <v>2612.72</v>
+        <v>3152.92</v>
       </c>
     </row>
     <row r="25">
@@ -1114,10 +1114,10 @@
         <v>0</v>
       </c>
       <c r="F27" t="str">
-        <v>0.467741501138221321</v>
+        <v>0.002418018646897028</v>
       </c>
       <c r="G27" t="str">
-        <v>465958.85</v>
+        <v>4590.86</v>
       </c>
     </row>
     <row r="28">
@@ -1137,10 +1137,10 @@
         <v>0</v>
       </c>
       <c r="F28" t="str">
-        <v>0.004789194341220858</v>
+        <v>0.007102039569921058</v>
       </c>
       <c r="G28" t="str">
-        <v>1476.14</v>
+        <v>2410.03</v>
       </c>
     </row>
     <row r="29">
@@ -1160,10 +1160,10 @@
         <v>0</v>
       </c>
       <c r="F29" t="str">
-        <v>0.000339263285881932</v>
+        <v>0.003966212891232665</v>
       </c>
       <c r="G29" t="str">
-        <v>276.54</v>
+        <v>1873.17</v>
       </c>
     </row>
     <row r="30">
@@ -1183,10 +1183,10 @@
         <v>0</v>
       </c>
       <c r="F30" t="str">
-        <v>0.003838891268915371</v>
+        <v>0.005691268976051839</v>
       </c>
       <c r="G30" t="str">
-        <v>856.53</v>
+        <v>2880.65</v>
       </c>
     </row>
     <row r="31">
@@ -1206,10 +1206,10 @@
         <v>0</v>
       </c>
       <c r="F31" t="str">
-        <v>11.43050771171794301</v>
+        <v>0.00272531448009951</v>
       </c>
       <c r="G31" t="str">
-        <v>5439524.2</v>
+        <v>1430.57</v>
       </c>
     </row>
     <row r="32">
@@ -1252,10 +1252,10 @@
         <v>0</v>
       </c>
       <c r="F33" t="str">
-        <v>0.455408184573896365</v>
+        <v>0.015823245848571587</v>
       </c>
       <c r="G33" t="str">
-        <v>470884.78</v>
+        <v>12614.43</v>
       </c>
     </row>
     <row r="34">
@@ -1275,10 +1275,10 @@
         <v>0</v>
       </c>
       <c r="F34" t="str">
-        <v>0.000549959731009076</v>
+        <v>0.000011114592899426</v>
       </c>
       <c r="G34" t="str">
-        <v>564.8</v>
+        <v>12.65</v>
       </c>
     </row>
     <row r="35">
@@ -1298,10 +1298,10 @@
         <v>0</v>
       </c>
       <c r="F35" t="str">
-        <v>0.242282136034294989</v>
+        <v>0.016857539829686085</v>
       </c>
       <c r="G35" t="str">
-        <v>236545.63</v>
+        <v>13988.78</v>
       </c>
     </row>
     <row r="36">
@@ -1321,10 +1321,10 @@
         <v>0</v>
       </c>
       <c r="F36" t="str">
-        <v>0.017201531372746433</v>
+        <v>0.001766955158360452</v>
       </c>
       <c r="G36" t="str">
-        <v>7198.38</v>
+        <v>3093.36</v>
       </c>
     </row>
     <row r="37">
@@ -1344,10 +1344,10 @@
         <v>0</v>
       </c>
       <c r="F37" t="str">
-        <v>0.171147566728327713</v>
+        <v>0.000023063182660471</v>
       </c>
       <c r="G37" t="str">
-        <v>168910.46</v>
+        <v>461.17</v>
       </c>
     </row>
     <row r="38">
@@ -1367,10 +1367,10 @@
         <v>0</v>
       </c>
       <c r="F38" t="str">
-        <v>0.134171849510780068</v>
+        <v>0.002789855269261671</v>
       </c>
       <c r="G38" t="str">
-        <v>133335.02</v>
+        <v>2926.24</v>
       </c>
     </row>
     <row r="39">
@@ -1390,10 +1390,10 @@
         <v>0</v>
       </c>
       <c r="F39" t="str">
-        <v>0.003700128984839755</v>
+        <v>0.001362119460166577</v>
       </c>
       <c r="G39" t="str">
-        <v>4173.22</v>
+        <v>2555.82</v>
       </c>
     </row>
     <row r="40">
@@ -1413,10 +1413,10 @@
         <v>0</v>
       </c>
       <c r="F40" t="str">
-        <v>0.129752119150991563</v>
+        <v>0.001363782155033188</v>
       </c>
       <c r="G40" t="str">
-        <v>131410.97</v>
+        <v>865.82</v>
       </c>
     </row>
     <row r="41">
@@ -1459,10 +1459,10 @@
         <v>0</v>
       </c>
       <c r="F42" t="str">
-        <v>0.672632583778337709</v>
+        <v>0.000024499472188667</v>
       </c>
       <c r="G42" t="str">
-        <v>684684.93</v>
+        <v>3668.12</v>
       </c>
     </row>
     <row r="43">
@@ -1482,7 +1482,7 @@
         <v>0</v>
       </c>
       <c r="F43" t="str">
-        <v>0</v>
+        <v>0.003774514860781313</v>
       </c>
       <c r="G43" t="str">
         <v>0</v>
@@ -1505,10 +1505,10 @@
         <v>0</v>
       </c>
       <c r="F44" t="str">
-        <v>0.004349679582553498</v>
+        <v>0.002694559931617619</v>
       </c>
       <c r="G44" t="str">
-        <v>22072.16</v>
+        <v>11235.91</v>
       </c>
     </row>
     <row r="45">
@@ -1574,10 +1574,10 @@
         <v>352296930353674</v>
       </c>
       <c r="F47" t="str">
-        <v>0.012208494365720498</v>
+        <v>0.01213908628442389</v>
       </c>
       <c r="G47" t="str">
-        <v>7804.17</v>
+        <v>6101.05</v>
       </c>
     </row>
     <row r="48">
@@ -1600,7 +1600,7 @@
         <v>0.016698632900169415</v>
       </c>
       <c r="G48" t="str">
-        <v>8571.52</v>
+        <v>8041.67</v>
       </c>
     </row>
     <row r="49">
@@ -1643,10 +1643,10 @@
         <v>0</v>
       </c>
       <c r="F50" t="str">
-        <v>0.46792365029496645</v>
+        <v>0.008911991647473406</v>
       </c>
       <c r="G50" t="str">
-        <v>466571.55</v>
+        <v>11838.38</v>
       </c>
     </row>
     <row r="51">
@@ -1666,10 +1666,10 @@
         <v>0</v>
       </c>
       <c r="F51" t="str">
-        <v>0.263195449253505377</v>
+        <v>0.000974441702683132</v>
       </c>
       <c r="G51" t="str">
-        <v>266498.54</v>
+        <v>1687.82</v>
       </c>
     </row>
     <row r="52">
@@ -1712,10 +1712,10 @@
         <v>0</v>
       </c>
       <c r="F53" t="str">
-        <v>0.015050067508017382</v>
+        <v>0</v>
       </c>
       <c r="G53" t="str">
-        <v>12508.79</v>
+        <v>1777.3</v>
       </c>
     </row>
     <row r="54">
@@ -1735,10 +1735,10 @@
         <v>0</v>
       </c>
       <c r="F54" t="str">
-        <v>0.037608045225955247</v>
+        <v>0.000117240627169197</v>
       </c>
       <c r="G54" t="str">
-        <v>40569.61</v>
+        <v>2770.77</v>
       </c>
     </row>
     <row r="55">
@@ -1781,10 +1781,10 @@
         <v>0</v>
       </c>
       <c r="F56" t="str">
-        <v>0.272993883766082745</v>
+        <v>0.002300783678480231</v>
       </c>
       <c r="G56" t="str">
-        <v>279775.07</v>
+        <v>3745.26</v>
       </c>
     </row>
     <row r="57">
@@ -11230,7 +11230,7 @@
         <v>1847.77</v>
       </c>
       <c r="D3" t="str">
-        <v>45.5</v>
+        <v>3405.92</v>
       </c>
       <c r="E3" t="str">
         <v>366483</v>
@@ -11247,7 +11247,7 @@
         <v>902.49</v>
       </c>
       <c r="D4" t="str">
-        <v>21.41</v>
+        <v>1602.81</v>
       </c>
       <c r="E4" t="str">
         <v>172465</v>
@@ -11264,7 +11264,7 @@
         <v>0.08</v>
       </c>
       <c r="D5" t="str">
-        <v>0</v>
+        <v>0.14</v>
       </c>
       <c r="E5" t="str">
         <v>16</v>
@@ -11281,7 +11281,7 @@
         <v>333.74</v>
       </c>
       <c r="D6" t="str">
-        <v>8.28</v>
+        <v>620.32</v>
       </c>
       <c r="E6" t="str">
         <v>66748</v>
@@ -11298,7 +11298,7 @@
         <v>14828.61</v>
       </c>
       <c r="D7" t="str">
-        <v>368.2</v>
+        <v>27562.06</v>
       </c>
       <c r="E7" t="str">
         <v>2965722</v>
@@ -11315,7 +11315,7 @@
         <v>749.34</v>
       </c>
       <c r="D8" t="str">
-        <v>17.58</v>
+        <v>1316.05</v>
       </c>
       <c r="E8" t="str">
         <v>141610</v>
@@ -11329,13 +11329,13 @@
         <v>0.002620746656338624</v>
       </c>
       <c r="C9" t="str">
-        <v>2571.06</v>
+        <v>2508.68</v>
       </c>
       <c r="D9" t="str">
-        <v>60.06</v>
+        <v>4438.32</v>
       </c>
       <c r="E9" t="str">
-        <v>483809</v>
+        <v>477571</v>
       </c>
     </row>
     <row r="10">
@@ -11366,7 +11366,7 @@
         <v>1114.38</v>
       </c>
       <c r="D11" t="str">
-        <v>27.63</v>
+        <v>2068.83</v>
       </c>
       <c r="E11" t="str">
         <v>222610</v>
@@ -11383,7 +11383,7 @@
         <v>14921.53</v>
       </c>
       <c r="D12" t="str">
-        <v>370.51</v>
+        <v>27734.77</v>
       </c>
       <c r="E12" t="str">
         <v>2984306</v>
@@ -11400,7 +11400,7 @@
         <v>140996.46</v>
       </c>
       <c r="D13" t="str">
-        <v>3501.04</v>
+        <v>262071.32</v>
       </c>
       <c r="E13" t="str">
         <v>28199292</v>
@@ -11411,16 +11411,16 @@
         <v>0x2fe6f7c52EccC8Fea03289EC10213033a7c364b7</v>
       </c>
       <c r="B14" t="str">
-        <v>36.938717697481499407</v>
+        <v>0.184406515513322905</v>
       </c>
       <c r="C14" t="str">
-        <v>19874889.12</v>
+        <v>158139.53</v>
       </c>
       <c r="D14" t="str">
-        <v>643464.88</v>
+        <v>295216.35</v>
       </c>
       <c r="E14" t="str">
-        <v>5182814984</v>
+        <v>31765750</v>
       </c>
     </row>
     <row r="15">
@@ -11434,7 +11434,7 @@
         <v>3562.55</v>
       </c>
       <c r="D15" t="str">
-        <v>88.46</v>
+        <v>6621.74</v>
       </c>
       <c r="E15" t="str">
         <v>712510</v>
@@ -11451,7 +11451,7 @@
         <v>4591.91</v>
       </c>
       <c r="D16" t="str">
-        <v>109.76</v>
+        <v>8216.27</v>
       </c>
       <c r="E16" t="str">
         <v>884084</v>
@@ -11462,16 +11462,16 @@
         <v>0x93Cf0a22a26895650A8AaE960Bf85a01ec6A551C</v>
       </c>
       <c r="B17" t="str">
-        <v>0.003838891268915371</v>
+        <v>0.005691268976051839</v>
       </c>
       <c r="C17" t="str">
-        <v>856.53</v>
+        <v>2880.65</v>
       </c>
       <c r="D17" t="str">
-        <v>51.86</v>
+        <v>7252.48</v>
       </c>
       <c r="E17" t="str">
-        <v>417730</v>
+        <v>780379</v>
       </c>
     </row>
     <row r="18">
@@ -11479,16 +11479,16 @@
         <v>0x69eC896E75aBFAf94680c84777be23E510e9df8c</v>
       </c>
       <c r="B18" t="str">
-        <v>0.000549959731009076</v>
+        <v>0.000011114592899426</v>
       </c>
       <c r="C18" t="str">
-        <v>564.8</v>
+        <v>12.65</v>
       </c>
       <c r="D18" t="str">
-        <v>12.91</v>
+        <v>20.68</v>
       </c>
       <c r="E18" t="str">
-        <v>104053</v>
+        <v>2226</v>
       </c>
     </row>
   </sheetData>

</xml_diff>